<commit_message>
2018-12-06 Przygotowanie (wszystkich) operacji dla modelu Country(Państwo)
</commit_message>
<xml_diff>
--- a/system.xlsx
+++ b/system.xlsx
@@ -348,7 +348,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -366,7 +366,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>43439</v>
+        <v>43438</v>
       </c>
       <c r="B2" s="2">
         <v>116103</v>
@@ -374,7 +374,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>43440</v>
+        <v>43439</v>
       </c>
       <c r="B3" s="2">
         <v>105117</v>
@@ -384,68 +384,72 @@
         <v>0.90537712203819021</v>
       </c>
       <c r="D3" s="3">
-        <f>C3/$B$2</f>
-        <v>7.798051058441128E-6</v>
+        <f>B3/$B$2</f>
+        <v>0.90537712203819021</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="1">
+        <v>43440</v>
+      </c>
+      <c r="B4" s="2">
+        <v>88603</v>
+      </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:C8" si="0">B4/B3</f>
-        <v>0</v>
+        <v>0.84289886507415546</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:D8" si="1">C4/$B$2</f>
-        <v>0</v>
+        <f>B4/$B$2</f>
+        <v>0.76314134863009564</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D5" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C5" s="3">
+        <f t="shared" ref="C5:C8" si="1">B5/B4</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D8" si="2">B5/$B$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D8" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2019-02-18 Zmiana stron w widoku index dla modelu Club
</commit_message>
<xml_diff>
--- a/system.xlsx
+++ b/system.xlsx
@@ -348,7 +348,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,7 +396,7 @@
         <v>88603</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" ref="C4:C8" si="0">B4/B3</f>
+        <f t="shared" ref="C4" si="0">B4/B3</f>
         <v>0.84289886507415546</v>
       </c>
       <c r="D4" s="3">
@@ -405,23 +405,27 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="1">
+        <v>43506</v>
+      </c>
+      <c r="B5" s="2">
+        <v>78055</v>
+      </c>
       <c r="C5" s="3">
         <f t="shared" ref="C5:C8" si="1">B5/B4</f>
-        <v>0</v>
+        <v>0.88095211223096281</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ref="D5:D8" si="2">B5/$B$2</f>
-        <v>0</v>
+        <v>0.67229098300646839</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="3" t="e">
+      <c r="C6" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="2"/>

</xml_diff>